<commit_message>
did more analysis, took fsr S3 calibration curve test data
</commit_message>
<xml_diff>
--- a/data/FSR_N1/stability/FSR_N1 Stability Data.xlsx
+++ b/data/FSR_N1/stability/FSR_N1 Stability Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amro365-my.sharepoint.com/personal/pr19556_appliedmed_com/Documents/Desktop/FSR/data/FSR_N1/stability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr19556\OneDrive - Applied Medical\Desktop\FSR\data\FSR_N1\stability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{FCD01CB3-A679-4E48-AC6D-BEC61BD358C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{422BEC8A-A57A-4639-9D6E-798C95D0124B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE80AA6-6CCF-4C8D-A2C6-26C251FC4D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5010" yWindow="6315" windowWidth="21600" windowHeight="12735" xr2:uid="{05FAEE67-03BB-4EED-BB39-2994B23103BF}"/>
+    <workbookView xWindow="3330" yWindow="3315" windowWidth="21600" windowHeight="12735" xr2:uid="{05FAEE67-03BB-4EED-BB39-2994B23103BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>FSR</t>
   </si>
@@ -71,7 +71,19 @@
     <t>FSR_N1_StabilityQuick(5.00lbf)</t>
   </si>
   <si>
-    <t>FSR_N1_Stability(5.00lbf)_Filtered</t>
+    <t>FSR_N1_Stability(5.00lbf)_20Filtered</t>
+  </si>
+  <si>
+    <t>FSR_N1_Stability(5.00lbf)_100Filtered</t>
+  </si>
+  <si>
+    <t>FSR_N1_Stability(5.00lbf)_50Filtered</t>
+  </si>
+  <si>
+    <t>Removed all Error &lt; 100%</t>
+  </si>
+  <si>
+    <t>Removed all Error &lt; 50%</t>
   </si>
 </sst>
 </file>
@@ -434,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F91B404-E44C-43FD-8798-D46178A2E488}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -529,6 +541,53 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>28.24</v>
+      </c>
+      <c r="D4">
+        <v>95.02</v>
+      </c>
+      <c r="E4">
+        <v>3.18</v>
+      </c>
+      <c r="F4">
+        <v>6.8650000000000002</v>
+      </c>
+      <c r="G4">
+        <v>379</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>